<commit_message>
Consolidate ISIC codes for most IO files
</commit_message>
<xml_diff>
--- a/InputData/io-model/IRoND/Interest Rate on National Debt.xlsx
+++ b/InputData/io-model/IRoND/Interest Rate on National Debt.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adolg\Dropbox\Energy Innovation IO\Deliverable IO files\EU\IRoND\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-eu\InputData\io-model\IRoND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{836135CD-F76F-4CE3-B781-B2A35DD31E11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="24195" windowHeight="20145" xr2:uid="{FD6B2E56-8C90-4A74-8ECD-784255639694}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="24195" windowHeight="20145"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -344,12 +343,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.##########"/>
     <numFmt numFmtId="165" formatCode="#,##0.0"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -569,7 +569,6 @@
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -577,13 +576,14 @@
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma 2" xfId="4" xr:uid="{3EFC5451-F535-4DDA-A6CA-150E87B768C9}"/>
+    <cellStyle name="Comma 2" xfId="4"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{340DD504-94F2-4B51-A4FC-491DD40A12E8}"/>
-    <cellStyle name="Percent 2" xfId="3" xr:uid="{52A908B6-4FE9-48FF-AE44-4527EBF9FFF4}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Percent 2" xfId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -943,7 +943,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2B31597-ACEC-4497-8C1B-442FAA403726}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -953,17 +953,17 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -971,52 +971,52 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2">
         <v>2021</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9" s="2">
         <v>2021</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" s="3" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="7"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -1024,7 +1024,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="7" t="s">
         <v>96</v>
       </c>
@@ -1034,7 +1034,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="7" t="s">
         <v>97</v>
       </c>
@@ -1044,14 +1044,14 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18" s="5"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="7" t="s">
         <v>98</v>
       </c>
@@ -1061,7 +1061,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="7" t="s">
         <v>99</v>
       </c>
@@ -1071,7 +1071,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
@@ -1081,7 +1081,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1" xr:uid="{758075EA-DE0E-4A0B-B9F2-3CBE1217E254}"/>
+    <hyperlink ref="B11" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -1089,7 +1089,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66BF0FAF-A2E1-44B1-852B-BD0E28BF0055}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1099,23 +1099,23 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="41.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="19.86328125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="10.3984375" style="8" customWidth="1"/>
+    <col min="3" max="3" width="41.73046875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="17.73046875" style="8" customWidth="1"/>
+    <col min="5" max="5" width="17.265625" style="8" customWidth="1"/>
+    <col min="6" max="6" width="6.265625" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" s="11" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" s="10" t="s">
         <v>27</v>
       </c>
@@ -1123,28 +1123,28 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
-      <c r="K8" s="36"/>
-      <c r="L8" s="36"/>
-      <c r="M8" s="36"/>
-      <c r="N8" s="36"/>
-      <c r="O8" s="36"/>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="35"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="35"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
+      <c r="M8" s="35"/>
+      <c r="N8" s="35"/>
+      <c r="O8" s="35"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" s="12" t="s">
         <v>23</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" s="12" t="s">
         <v>22</v>
       </c>
@@ -1160,17 +1160,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B13" s="13" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="C14" s="12" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.45">
       <c r="B17" s="10" t="s">
         <v>13</v>
       </c>
@@ -1209,9 +1209,9 @@
     <mergeCell ref="B8:O8"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" xr:uid="{A0288D83-DBB5-49D0-A4FB-DF39FA0B11C8}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{D615B1FF-C5C9-4B17-AA16-4B58ED8B9834}"/>
-    <hyperlink ref="B17" location="'Sheet 1'!A1" display="Sheet 1" xr:uid="{8B8310EA-EAED-48BA-95C3-72D8D5DC3150}"/>
+    <hyperlink ref="A7" r:id="rId1"/>
+    <hyperlink ref="B7" r:id="rId2"/>
+    <hyperlink ref="B17" location="'Sheet 1'!A1" display="Sheet 1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>
@@ -1219,7 +1219,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBA2D75-E6BF-4EB5-8450-EDCD39D1FEC9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1229,20 +1229,20 @@
       <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="30.28515625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="37.5703125" style="8" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.1328125" style="8"/>
+    <col min="2" max="2" width="30.265625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="37.59765625" style="8" customWidth="1"/>
+    <col min="4" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B2" s="16" t="s">
         <v>73</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B3" s="15" t="s">
         <v>71</v>
       </c>
@@ -1258,7 +1258,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B4" s="12" t="s">
         <v>17</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B5" s="9" t="s">
         <v>36</v>
       </c>
@@ -1274,7 +1274,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B6" s="12" t="s">
         <v>36</v>
       </c>
@@ -1282,7 +1282,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B7" s="9" t="s">
         <v>36</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B8" s="12" t="s">
         <v>36</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B9" s="9" t="s">
         <v>36</v>
       </c>
@@ -1306,7 +1306,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B10" s="12" t="s">
         <v>36</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B11" s="9" t="s">
         <v>36</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B12" s="12" t="s">
         <v>36</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B14" s="12" t="s">
         <v>36</v>
       </c>
@@ -1346,7 +1346,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B15" s="9" t="s">
         <v>36</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B16" s="12" t="s">
         <v>36</v>
       </c>
@@ -1362,7 +1362,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B17" s="9" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B18" s="12" t="s">
         <v>36</v>
       </c>
@@ -1378,7 +1378,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B19" s="9" t="s">
         <v>36</v>
       </c>
@@ -1386,7 +1386,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B20" s="12" t="s">
         <v>36</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B21" s="9" t="s">
         <v>36</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B22" s="12" t="s">
         <v>36</v>
       </c>
@@ -1410,7 +1410,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B23" s="9" t="s">
         <v>36</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B24" s="12" t="s">
         <v>36</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B25" s="9" t="s">
         <v>36</v>
       </c>
@@ -1434,7 +1434,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B26" s="12" t="s">
         <v>36</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B27" s="9" t="s">
         <v>36</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B28" s="12" t="s">
         <v>36</v>
       </c>
@@ -1458,7 +1458,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B29" s="9" t="s">
         <v>36</v>
       </c>
@@ -1466,7 +1466,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B30" s="12" t="s">
         <v>36</v>
       </c>
@@ -1474,7 +1474,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B31" s="9" t="s">
         <v>36</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B32" s="12" t="s">
         <v>36</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B33" s="9" t="s">
         <v>36</v>
       </c>
@@ -1498,7 +1498,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B34" s="12" t="s">
         <v>36</v>
       </c>
@@ -1506,7 +1506,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B35" s="9" t="s">
         <v>36</v>
       </c>
@@ -1514,7 +1514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B36" s="12" t="s">
         <v>36</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B37" s="9" t="s">
         <v>36</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B38" s="12" t="s">
         <v>36</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B39" s="9" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1546,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B40" s="12" t="s">
         <v>16</v>
       </c>
@@ -1554,7 +1554,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B41" s="9" t="s">
         <v>15</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B42" s="12" t="s">
         <v>14</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B43" s="9" t="s">
         <v>30</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B44" s="12" t="s">
         <v>30</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B45" s="9" t="s">
         <v>30</v>
       </c>
@@ -1594,7 +1594,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B46" s="12" t="s">
         <v>30</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.45">
       <c r="B47" s="9" t="s">
         <v>30</v>
       </c>
@@ -1616,7 +1616,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E75E06C-EC73-49C1-9723-3D32FBCCD6D9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -1630,10 +1630,10 @@
       <selection pane="bottomRight" activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="11.45" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="29.85546875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="43.28515625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="29.86328125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="43.265625" style="8" customWidth="1"/>
     <col min="3" max="3" width="5" style="8" customWidth="1"/>
     <col min="4" max="4" width="18" style="8" customWidth="1"/>
     <col min="5" max="5" width="5" style="8" customWidth="1"/>
@@ -1641,17 +1641,17 @@
     <col min="7" max="7" width="5" style="8" customWidth="1"/>
     <col min="8" max="8" width="16" style="8" customWidth="1"/>
     <col min="9" max="9" width="5" style="8" customWidth="1"/>
-    <col min="10" max="10" width="19.85546875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="19.86328125" style="8" customWidth="1"/>
     <col min="11" max="11" width="5" style="8" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="8"/>
+    <col min="12" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>82</v>
       </c>
@@ -1659,7 +1659,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>81</v>
       </c>
@@ -1670,12 +1670,12 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C4" s="8">
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="13" t="s">
         <v>15</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>1.8220000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="13" t="s">
         <v>16</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="13" t="s">
         <v>17</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>-0.25900000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8" s="13" t="s">
         <v>14</v>
       </c>
@@ -1707,45 +1707,45 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C9" s="8">
         <v>0.104</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>34</v>
       </c>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37" t="s">
+      <c r="C10" s="36"/>
+      <c r="D10" s="36" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="37" t="s">
+      <c r="E10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="G10" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="H10" s="37" t="s">
+      <c r="G10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="I10" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="J10" s="37" t="s">
+      <c r="I10" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="J10" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="26" t="s">
         <v>79</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="19" t="s">
         <v>70</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="19" t="s">
         <v>69</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="19" t="s">
         <v>68</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="19" t="s">
         <v>67</v>
       </c>
@@ -1920,7 +1920,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="19" t="s">
         <v>66</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="19" t="s">
         <v>65</v>
       </c>
@@ -1990,7 +1990,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="19" t="s">
         <v>64</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="19" t="s">
         <v>63</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="19" t="s">
         <v>62</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="19" t="s">
         <v>61</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="19" t="s">
         <v>60</v>
       </c>
@@ -2165,7 +2165,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23" s="19" t="s">
         <v>59</v>
       </c>
@@ -2200,7 +2200,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24" s="19" t="s">
         <v>58</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25" s="19" t="s">
         <v>57</v>
       </c>
@@ -2270,7 +2270,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26" s="19" t="s">
         <v>56</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="19" t="s">
         <v>55</v>
       </c>
@@ -2340,7 +2340,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A28" s="19" t="s">
         <v>54</v>
       </c>
@@ -2375,7 +2375,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="11.45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A29" s="19" t="s">
         <v>53</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A30" s="19" t="s">
         <v>52</v>
       </c>
@@ -2445,7 +2445,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="19" t="s">
         <v>51</v>
       </c>
@@ -2480,7 +2480,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="19" t="s">
         <v>50</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A33" s="19" t="s">
         <v>49</v>
       </c>
@@ -2550,7 +2550,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="19" t="s">
         <v>48</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="19" t="s">
         <v>47</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="19" t="s">
         <v>46</v>
       </c>
@@ -2655,7 +2655,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A37" s="19" t="s">
         <v>45</v>
       </c>
@@ -2690,7 +2690,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A38" s="19" t="s">
         <v>44</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A39" s="19" t="s">
         <v>43</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A40" s="19" t="s">
         <v>42</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A41" s="19" t="s">
         <v>41</v>
       </c>
@@ -2830,7 +2830,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A42" s="19" t="s">
         <v>40</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A43" s="19" t="s">
         <v>39</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A44" s="19" t="s">
         <v>38</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A45" s="19" t="s">
         <v>37</v>
       </c>
@@ -2970,7 +2970,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A46" s="19" t="s">
         <v>35</v>
       </c>
@@ -3005,12 +3005,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A48" s="13" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A49" s="13" t="s">
         <v>76</v>
       </c>
@@ -3031,7 +3031,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B707EDC8-4431-49AE-A085-E3FA459AC7D0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -3041,24 +3041,24 @@
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="8"/>
-    <col min="2" max="2" width="43.28515625" style="8" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="1" width="9.1328125" style="8"/>
+    <col min="2" max="2" width="43.265625" style="8" customWidth="1"/>
+    <col min="3" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B2" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B4" s="19" t="s">
         <v>63</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>5.7000000000000002E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B5" s="19" t="s">
         <v>62</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B6" s="19" t="s">
         <v>61</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>1.8220000000000001</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B7" s="19" t="s">
         <v>60</v>
       </c>
@@ -3090,7 +3090,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B8" s="19" t="s">
         <v>59</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>-0.25900000000000001</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B9" s="19" t="s">
         <v>58</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B10" s="19" t="s">
         <v>57</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B11" s="19" t="s">
         <v>56</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B12" s="19" t="s">
         <v>55</v>
       </c>
@@ -3134,7 +3134,7 @@
         <v>0.39700000000000002</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B13" s="19" t="s">
         <v>54</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B14" s="19" t="s">
         <v>53</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>0.67300000000000004</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B15" s="19" t="s">
         <v>52</v>
       </c>
@@ -3158,7 +3158,7 @@
         <v>0.746</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B16" s="19" t="s">
         <v>51</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>0.40100000000000002</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B17" s="19" t="s">
         <v>50</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>0.54900000000000004</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B18" s="19" t="s">
         <v>49</v>
       </c>
@@ -3182,7 +3182,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B19" s="19" t="s">
         <v>48</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B20" s="19" t="s">
         <v>47</v>
       </c>
@@ -3202,7 +3202,7 @@
         <v>2.6349999999999998</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B21" s="19" t="s">
         <v>46</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>0.47299999999999998</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B22" s="19" t="s">
         <v>45</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>-0.20399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B23" s="19" t="s">
         <v>44</v>
       </c>
@@ -3226,7 +3226,7 @@
         <v>-3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B24" s="19" t="s">
         <v>43</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>1.4710000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B25" s="19" t="s">
         <v>42</v>
       </c>
@@ -3242,7 +3242,7 @@
         <v>0.377</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B26" s="19" t="s">
         <v>41</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B27" s="19" t="s">
         <v>40</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>7.0999999999999994E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B28" s="19" t="s">
         <v>39</v>
       </c>
@@ -3266,7 +3266,7 @@
         <v>-0.08</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B29" s="19" t="s">
         <v>38</v>
       </c>
@@ -3274,7 +3274,7 @@
         <v>-8.5999999999999993E-2</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B30" s="19" t="s">
         <v>37</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>0.375</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
       <c r="B31" s="19" t="s">
         <v>35</v>
       </c>
@@ -3296,7 +3296,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F6E3BBB-DF65-4FB1-A055-F01BF58D7B1F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
@@ -3306,14 +3306,14 @@
       <selection activeCell="I53" sqref="I53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="3" width="9.140625" style="8"/>
-    <col min="4" max="5" width="13.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="8"/>
+    <col min="1" max="3" width="9.1328125" style="8"/>
+    <col min="4" max="5" width="13.265625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1328125" style="8"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.45">
       <c r="C4" s="8" t="s">
         <v>92</v>
       </c>
@@ -3324,7 +3324,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B5" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B4</f>
         <v>Belgium</v>
@@ -3342,7 +3342,7 @@
         <v>26616.788400000001</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B6" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B5</f>
         <v>Bulgaria</v>
@@ -3360,7 +3360,7 @@
         <v>1856.925</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B7" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B6</f>
         <v>Czechia</v>
@@ -3378,7 +3378,7 @@
         <v>124663.973</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B8" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B7</f>
         <v>Denmark</v>
@@ -3396,7 +3396,7 @@
         <v>3856.3064999999997</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B9" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B8</f>
         <v>Germany (until 1990 former territory of the FRG)</v>
@@ -3414,7 +3414,7 @@
         <v>-532805.89040000003</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B10" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B9</f>
         <v>Estonia</v>
@@ -3432,7 +3432,7 @@
         <v>769.8438000000001</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B11" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B10</f>
         <v>Ireland</v>
@@ -3450,7 +3450,7 @@
         <v>21236.581599999998</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B12" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B11</f>
         <v>Greece</v>
@@ -3468,7 +3468,7 @@
         <v>299951.23200000002</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B13" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B12</f>
         <v>Spain</v>
@@ -3486,7 +3486,7 @@
         <v>471977.02300000004</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B14" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B13</f>
         <v>France</v>
@@ -3504,7 +3504,7 @@
         <v>-11900.205</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B15" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B14</f>
         <v>Croatia</v>
@@ -3522,7 +3522,7 @@
         <v>26498.971200000004</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B16" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B15</f>
         <v>Italy</v>
@@ -3540,7 +3540,7 @@
         <v>1797788.3093999999</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B17" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B16</f>
         <v>Cyprus</v>
@@ -3558,7 +3558,7 @@
         <v>8404.1580000000013</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B18" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B17</f>
         <v>Latvia</v>
@@ -3576,7 +3576,7 @@
         <v>6174.3834000000006</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B19" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B18</f>
         <v>Lithuania</v>
@@ -3594,7 +3594,7 @@
         <v>1752.3900000000003</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B20" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B19</f>
         <v>Luxembourg</v>
@@ -3612,7 +3612,7 @@
         <v>-1435.1092500000002</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B21" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B20</f>
         <v>Hungary</v>
@@ -3630,7 +3630,7 @@
         <v>247751.39549999998</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B22" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B21</f>
         <v>Malta</v>
@@ -3648,7 +3648,7 @@
         <v>2699.5056</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B23" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B22</f>
         <v>Netherlands</v>
@@ -3666,7 +3666,7 @@
         <v>-80512.679999999993</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B24" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B23</f>
         <v>Austria</v>
@@ -3684,7 +3684,7 @@
         <v>-10653.060600000001</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B25" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B24</f>
         <v>Poland</v>
@@ -3702,7 +3702,7 @@
         <v>361250.23940000002</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B26" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B25</f>
         <v>Portugal</v>
@@ -3720,7 +3720,7 @@
         <v>94244.382700000002</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B26</f>
         <v>Romania</v>
@@ -3738,7 +3738,7 @@
         <v>242156.81000000003</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B28" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B27</f>
         <v>Slovenia</v>
@@ -3756,7 +3756,7 @@
         <v>2253.8523999999998</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B28</f>
         <v>Slovakia</v>
@@ -3774,7 +3774,7 @@
         <v>-3638.84</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B30" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B29</f>
         <v>Finland</v>
@@ -3792,7 +3792,7 @@
         <v>-12258.353999999999</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B31" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B30</f>
         <v>Sweden</v>
@@ -3810,7 +3810,7 @@
         <v>63245.549999999996</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.45">
       <c r="B32" s="8" t="str">
         <f>'WGB.com 10Y Bond data'!B31</f>
         <v>United Kingdom</v>
@@ -3828,12 +3828,12 @@
         <v>1700361.8280000002</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.45">
       <c r="G33" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.45">
       <c r="B34" s="8" t="s">
         <v>88</v>
       </c>
@@ -3859,23 +3859,23 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C01F22F6-4878-43A7-B39F-16DF94601E91}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="4" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="15.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -3883,11 +3883,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="34">
+      <c r="B2" s="37">
         <f>'Debt IR calcs'!G34</f>
         <v>3.6515867657555849E-3</v>
       </c>

</xml_diff>